<commit_message>
bug fixing. First socialgroup for visit at household level should be 01.
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/location_registration.xlsx
+++ b/xforms/xlsforms/location_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-135" windowWidth="15600" windowHeight="11700" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="25605" yWindow="-135" windowWidth="15600" windowHeight="11700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>type</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Location registration</t>
-  </si>
-  <si>
-    <t>${locationId}</t>
   </si>
   <si>
     <t>deviceId</t>
@@ -1382,11 +1379,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1503,7 +1500,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1520,13 +1517,13 @@
     </row>
     <row r="5" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -1534,7 +1531,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
@@ -1613,10 +1610,10 @@
     </row>
     <row r="9" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1635,9 +1632,6 @@
       <c r="I10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -1675,16 +1669,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M13" s="5" t="b">
         <v>1</v>
@@ -2370,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2387,7 +2381,7 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -2401,7 +2395,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>